<commit_message>
Starting to adapt everything to the tractor
</commit_message>
<xml_diff>
--- a/Pin's Arduino MEGA.xlsx
+++ b/Pin's Arduino MEGA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/mb70069_uga_edu/Documents/100 - Corn_seed_orientation/100 - GitHub_MotorControl_CSO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_AD4DB114E441178AC67DF4866656CB18693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A471A319-0167-4133-9BCE-CAE4CC60E31F}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_AD4DB114E441178AC67DF4866656CB18693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C3B404-1762-4981-AE40-E6D47E6042B2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39990" yWindow="525" windowWidth="17280" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Arduino MEGA</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>RST</t>
+  </si>
+  <si>
+    <t>Cable from Tractor</t>
+  </si>
+  <si>
+    <t>CAN Low</t>
+  </si>
+  <si>
+    <t>CAN High</t>
+  </si>
+  <si>
+    <t>ECU Power</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>48 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -119,6 +140,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,16 +409,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F18"/>
+  <dimension ref="B3:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -502,6 +527,41 @@
         <v>13</v>
       </c>
     </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>